<commit_message>
Add search and filter for species
</commit_message>
<xml_diff>
--- a/server/temp/test.xlsx
+++ b/server/temp/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
   <si>
     <t>englishName</t>
   </si>
@@ -73,7 +73,7 @@
     <t>observations</t>
   </si>
   <si>
-    <t>Photos</t>
+    <t>photos</t>
   </si>
   <si>
     <t>Snow Partridge</t>
@@ -163,72 +163,15 @@
     <t>["images/Black Francolin.jpg"]</t>
   </si>
   <si>
-    <t>Tibetan Snowcock</t>
-  </si>
-  <si>
-    <t>Tetraogallus tibetanus</t>
-  </si>
-  <si>
-    <t>Tetraogallus</t>
-  </si>
-  <si>
-    <t>tibetanus</t>
-  </si>
-  <si>
-    <t>Gould, 1854</t>
-  </si>
-  <si>
-    <t>Snowcock</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>II</t>
-  </si>
-  <si>
-    <t>Common Quail</t>
-  </si>
-  <si>
-    <t>Coturnix coturnix</t>
+    <t>Japanese Quail</t>
+  </si>
+  <si>
+    <t>Coturnix japonica</t>
   </si>
   <si>
     <t>Coturnix</t>
   </si>
   <si>
-    <t>coturnix</t>
-  </si>
-  <si>
-    <t>(Linnaeus, 1758)</t>
-  </si>
-  <si>
-    <t>Quail</t>
-  </si>
-  <si>
-    <t>Passage migrant</t>
-  </si>
-  <si>
-    <t>Grassland</t>
-  </si>
-  <si>
-    <t>Japanese Quail</t>
-  </si>
-  <si>
-    <t>Coturnix japonica</t>
-  </si>
-  <si>
-    <t>japonica</t>
-  </si>
-  <si>
-    <t>Temminck and Schlegel, 1849</t>
-  </si>
-  <si>
-    <t>NT</t>
-  </si>
-  <si>
-    <t>Summer visitor</t>
-  </si>
-  <si>
     <t>Yellow-legged Buttonquail</t>
   </si>
   <si>
@@ -244,25 +187,10 @@
     <t>Turnix</t>
   </si>
   <si>
-    <t>tanki</t>
-  </si>
-  <si>
-    <t>Blyth, 1843</t>
-  </si>
-  <si>
-    <t>Buttonquail</t>
-  </si>
-  <si>
     <t>Barred Buttonquail</t>
   </si>
   <si>
     <t>Turnix suscitator</t>
-  </si>
-  <si>
-    <t>suscitator</t>
-  </si>
-  <si>
-    <t>(Gmelin, JF, 1789)</t>
   </si>
 </sst>
 </file>
@@ -272,8 +200,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -317,11 +245,71 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -333,21 +321,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -356,29 +329,52 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -386,76 +382,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -482,13 +410,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -500,25 +572,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -530,139 +590,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -743,15 +671,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -763,26 +682,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -820,8 +719,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -840,20 +739,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -863,130 +791,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1014,7 +942,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1334,13 +1264,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="1" width="24.2222222222222" customWidth="1"/>
     <col min="2" max="2" width="22.3333333333333" customWidth="1"/>
@@ -1588,228 +1518,87 @@
       <c r="E5" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="M5" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="R5" s="3"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="13" t="str">
-        <f>CONCATENATE("[images/",A5,".jpg]")</f>
-        <v>[images/Tibetan Snowcock.jpg]</v>
-      </c>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
     </row>
     <row r="6" spans="1:20">
       <c r="A6" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>62</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
-      <c r="M6" s="8" t="s">
-        <v>28</v>
-      </c>
+      <c r="M6" s="8"/>
       <c r="N6" s="8"/>
-      <c r="O6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="R6" s="3"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="13" t="str">
-        <f>CONCATENATE("[images/",A6,".jpg]")</f>
-        <v>[images/Common Quail.jpg]</v>
-      </c>
+      <c r="O6" s="8"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:20">
       <c r="A7" s="3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>62</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="8" t="s">
-        <v>69</v>
-      </c>
+      <c r="M7" s="8"/>
       <c r="N7" s="8"/>
-      <c r="O7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="R7" s="3" t="str">
-        <f t="shared" ref="R7:R9" si="0">CONCATENATE("[images/",A7,".jpg]")</f>
-        <v>[images/Japanese Quail.jpg]</v>
-      </c>
+      <c r="O7" s="8"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
     </row>
-    <row r="8" spans="1:18">
-      <c r="A8" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="R8" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>[images/Yellow-legged Buttonquail.jpg]</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
-      <c r="A9" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="R9" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>[images/Barred Buttonquail.jpg]</v>
-      </c>
-    </row>
-    <row r="10" ht="16" customHeight="1"/>
+    <row r="8" ht="16" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
download excel report of species
</commit_message>
<xml_diff>
--- a/server/temp/test.xlsx
+++ b/server/temp/test.xlsx
@@ -9155,7 +9155,7 @@
     <t>Alpine meadows</t>
   </si>
   <si>
-    <t>Smoky Warbler["images/Smoky Warbler.png"]</t>
+    <t>["images/Smoky Warbler.png"]</t>
   </si>
   <si>
     <t>Sulphur-bellied Warbler</t>
@@ -9230,7 +9230,7 @@
     <t>cantator</t>
   </si>
   <si>
-    <t>Y["images/ellow-vented Warbler.png"]</t>
+    <t>["images/ellow-vented Warbler.png"]</t>
   </si>
   <si>
     <t>Black-faced Warbler</t>
@@ -13853,8 +13853,8 @@
   <sheetPr/>
   <dimension ref="A1:T780"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q304" workbookViewId="0">
-      <selection activeCell="T327" sqref="T327"/>
+    <sheetView tabSelected="1" topLeftCell="Q757" workbookViewId="0">
+      <selection activeCell="T776" sqref="T776"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>

</xml_diff>